<commit_message>
working on fixed power or speed figure
</commit_message>
<xml_diff>
--- a/notebooks/basic functionality/application example.xlsx
+++ b/notebooks/basic functionality/application example.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
     <sheet name="speed-power" sheetId="2" r:id="rId2"/>
-    <sheet name="original speed-power data" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="original speed-power data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="292">
   <si>
     <t>6-4-6</t>
   </si>
@@ -839,9 +840,6 @@
     <t>load=1500t</t>
   </si>
   <si>
-    <t>load=2500t</t>
-  </si>
-  <si>
     <t>speed limit=4,47m/s=16,09km/h</t>
   </si>
   <si>
@@ -864,6 +862,42 @@
   </si>
   <si>
     <t>power limit=1622,27kW</t>
+  </si>
+  <si>
+    <t>2500payload</t>
+  </si>
+  <si>
+    <t>2500payload,3000load</t>
+  </si>
+  <si>
+    <t>1000payload,1500load</t>
+  </si>
+  <si>
+    <t>load=3000t</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>partial engine load</t>
+  </si>
+  <si>
+    <t>fix speed m/s</t>
+  </si>
+  <si>
+    <t>fix power  kW</t>
+  </si>
+  <si>
+    <t>h=6 full</t>
+  </si>
+  <si>
+    <t>h=4 full</t>
+  </si>
+  <si>
+    <t>h=6, 1500load</t>
+  </si>
+  <si>
+    <t>h=2.5, 1500load</t>
   </si>
 </sst>
 </file>
@@ -871,9 +905,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -909,8 +943,15 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -941,8 +982,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -950,31 +1003,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -984,9 +1043,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -994,9 +1053,40 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,20 +1108,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>706118</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>163668</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>96056</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1050,8 +1140,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4655818" y="2838450"/>
-          <a:ext cx="4551682" cy="3211668"/>
+          <a:off x="5308600" y="2895600"/>
+          <a:ext cx="4661706" cy="3289300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1329,7 +1419,7 @@
   <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1341,12 +1431,16 @@
     <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.36328125" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="22.54296875" customWidth="1"/>
     <col min="13" max="13" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
@@ -1406,11 +1500,17 @@
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -1420,10 +1520,10 @@
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="31" t="s">
-        <v>275</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1431,9 +1531,12 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>280</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1445,7 +1548,7 @@
     </row>
     <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1455,9 +1558,9 @@
     <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D8" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1467,7 +1570,7 @@
     <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1479,7 +1582,7 @@
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -1494,7 +1597,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="3" t="s">
@@ -1502,6 +1605,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>281</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -1518,7 +1624,7 @@
     </row>
     <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1528,9 +1634,9 @@
     <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D17" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1540,7 +1646,7 @@
     <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="7"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="5" t="s">
         <v>21</v>
       </c>
@@ -1552,7 +1658,7 @@
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1567,9 +1673,9 @@
         <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D22" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1577,16 +1683,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>282</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4"/>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -1596,9 +1705,9 @@
     <row r="26" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D26" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D26" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1608,7 +1717,7 @@
     <row r="27" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="7"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="5" t="s">
         <v>21</v>
       </c>
@@ -1630,19 +1739,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="27.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="9" customWidth="1"/>
     <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.90625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.26953125" style="3" bestFit="1" customWidth="1"/>
@@ -1650,92 +1759,92 @@
     <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30" t="s">
+    <row r="1" spans="1:14" s="10" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="F3" s="10" t="s">
+      <c r="D3" s="9"/>
+      <c r="F3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="8"/>
       <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="B4" s="18">
+      <c r="A4" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="B4" s="15">
         <v>94.619917291274803</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="16">
         <v>1.01306532663316</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="15">
         <v>3.6470351758793758</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="F4" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G4" s="8">
         <v>95.98</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="17">
         <v>1.01306532663316</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="20">
         <v>3.6470351758793758</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -1744,36 +1853,36 @@
       <c r="L4" s="3">
         <v>95.87</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="18">
         <v>1.01306532663316</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="19">
         <v>3.6470351758793758</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="15">
         <v>109.206761541059</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="16">
         <v>1.4894472361808999</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="15">
         <v>5.3620100502512402</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="F5" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="8">
         <v>113.18</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>1.4894472361808999</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="20">
         <v>5.3620100502512402</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -1782,230 +1891,239 @@
       <c r="L5" s="3">
         <v>112.66</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="18">
         <v>1.4894472361808999</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="19">
         <v>5.3620100502512402</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="18">
+      <c r="B6" s="15">
         <v>138.888710274706</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="16">
         <v>2.0055276381909501</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="15">
         <v>7.2198994974874209</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>148.07</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>2.0055276381909501</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="20">
         <v>7.2198994974874209</v>
       </c>
       <c r="L6" s="3">
         <v>146.69999999999999</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="18">
         <v>2.0055276381909501</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="19">
         <v>7.2198994974874209</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="18">
+    <row r="7" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="32"/>
+      <c r="B7" s="33">
         <v>182.952887615695</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="34">
         <v>2.4819095477386899</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="33">
         <v>8.9348743718592836</v>
       </c>
-      <c r="G7" s="10">
+      <c r="F7" s="36"/>
+      <c r="G7" s="36">
         <v>199.86</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="37">
         <v>2.4819095477386899</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="38">
         <v>8.9348743718592836</v>
       </c>
-      <c r="L7" s="3">
+      <c r="K7" s="39"/>
+      <c r="L7" s="39">
         <v>197.66</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="40">
         <v>2.4819095477386899</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="41">
         <v>8.9348743718592836</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="18">
+    <row r="8" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33">
         <v>253.78462040345201</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="34">
         <v>2.9979899497487401</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="33">
         <v>10.792763819095464</v>
       </c>
-      <c r="G8" s="10">
+      <c r="F8" s="36"/>
+      <c r="G8" s="36">
         <v>281.26</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="37">
         <v>2.9979899497487401</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="38">
         <v>10.792763819095464</v>
       </c>
-      <c r="L8" s="3">
+      <c r="K8" s="39"/>
+      <c r="L8" s="39">
         <v>311.11</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="40">
         <v>2.9979899497487401</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="41">
         <v>10.792763819095464</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="18">
+    <row r="9" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33">
         <v>352.26875986340798</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="34">
         <v>3.5140703517587899</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="33">
         <v>12.650653266331643</v>
       </c>
-      <c r="G9" s="10">
+      <c r="F9" s="36"/>
+      <c r="G9" s="36">
         <v>423.01</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="37">
         <v>3.5140703517587899</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="38">
         <v>12.650653266331643</v>
       </c>
-      <c r="L9" s="3">
+      <c r="K9" s="39"/>
+      <c r="L9" s="39">
         <v>721.61</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="40">
         <v>3.5140703517587899</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="41">
         <v>12.650653266331643</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="18">
+      <c r="B10" s="15">
         <v>518.14499428592205</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="16">
         <v>4.0301507537688401</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="15">
         <v>14.508542713567826</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="8">
         <v>767.72</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <v>4.0301507537688401</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="20">
         <v>14.508542713567826</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="23">
         <v>1622.27</v>
       </c>
-      <c r="M10" s="27">
+      <c r="M10" s="24">
         <v>3.87</v>
       </c>
-      <c r="N10" s="27">
+      <c r="N10" s="24">
         <f>M10*3.6</f>
         <v>13.932</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="18">
+      <c r="B11" s="15">
         <v>837.42056198015803</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="16">
         <v>4.5065326633165803</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>16.223517587939689</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="21">
         <v>1662.56</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="22">
         <v>4.47</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="22">
         <f>H11*3.6</f>
         <v>16.091999999999999</v>
       </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="22"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="28">
+      <c r="B12" s="25">
         <v>1743.2466559675099</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="26">
         <v>5.0226130653266301</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="25">
         <v>18.081407035175868</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="23"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="22"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="20"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D13" s="11"/>
-      <c r="I13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="I13" s="8"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D14" s="11"/>
-      <c r="I14" s="10"/>
+      <c r="D14" s="9"/>
+      <c r="I14" s="8"/>
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D15" s="11"/>
-      <c r="I15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="I15" s="8"/>
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="D16" s="11"/>
-      <c r="I16" s="10"/>
+      <c r="D16" s="9"/>
+      <c r="I16" s="8"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D17" s="11"/>
-      <c r="I17" s="10"/>
+      <c r="D17" s="9"/>
+      <c r="I17" s="8"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D18" s="11"/>
-      <c r="I18" s="10"/>
+      <c r="D18" s="9"/>
+      <c r="I18" s="8"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.35">
-      <c r="D19" s="11"/>
-      <c r="I19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="I19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2019,10 +2137,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1" s="44">
+        <v>3</v>
+      </c>
+      <c r="C1" s="44">
+        <v>3.5</v>
+      </c>
+      <c r="D1" s="44">
+        <v>4</v>
+      </c>
+      <c r="E1" s="44">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="43"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>284</v>
+      </c>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="47">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="47">
+        <v>0.75</v>
+      </c>
+      <c r="F7" s="47">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="44" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="45">
+        <v>175</v>
+      </c>
+      <c r="C8" s="45">
+        <v>525</v>
+      </c>
+      <c r="D8" s="45">
+        <v>875</v>
+      </c>
+      <c r="E8" s="45">
+        <v>1313</v>
+      </c>
+      <c r="F8" s="45">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q127"/>
   <sheetViews>
-    <sheetView topLeftCell="C94" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2039,7 +2334,7 @@
       <c r="C1">
         <v>0</v>
       </c>
-      <c r="D1" s="15">
+      <c r="D1" s="12">
         <v>8750911319076930</v>
       </c>
       <c r="E1" t="s">
@@ -2052,13 +2347,13 @@
       <c r="I1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>62</v>
       </c>
       <c r="P1" t="s">
         <v>173</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="11" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2066,7 +2361,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="12">
         <v>8752373047524240</v>
       </c>
       <c r="E2" t="s">
@@ -2076,19 +2371,19 @@
         <f t="shared" ref="F2:F65" si="0">D2/10000000000000</f>
         <v>875.23730475242405</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
+      <c r="B3" s="11"/>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <v>8754861508869450</v>
       </c>
       <c r="E3" t="s">
@@ -2098,19 +2393,19 @@
         <f t="shared" si="0"/>
         <v>875.48615088694498</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="11" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B4" s="14"/>
+      <c r="B4" s="11"/>
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>8758629985849390</v>
       </c>
       <c r="E4" t="s">
@@ -2120,19 +2415,19 @@
         <f t="shared" si="0"/>
         <v>875.86299858493896</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="11" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B5" s="14"/>
+      <c r="B5" s="11"/>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>876392585419736</v>
       </c>
       <c r="E5" t="s">
@@ -2142,19 +2437,19 @@
         <f t="shared" si="0"/>
         <v>87.639258541973604</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="11" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B6" s="14"/>
+      <c r="B6" s="11"/>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>877099184509031</v>
       </c>
       <c r="E6" t="s">
@@ -2164,19 +2459,19 @@
         <f t="shared" si="0"/>
         <v>87.709918450903103</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="11" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
+      <c r="B7" s="11"/>
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>8780066874937540</v>
       </c>
       <c r="E7" t="s">
@@ -2186,19 +2481,19 @@
         <f t="shared" si="0"/>
         <v>878.00668749375404</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="Q7" s="11" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
+      <c r="B8" s="11"/>
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>8791386631832680</v>
       </c>
       <c r="E8" t="s">
@@ -2208,19 +2503,19 @@
         <f t="shared" si="0"/>
         <v>879.13866318326802</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="Q8" s="11" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
+      <c r="B9" s="11"/>
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>8805184011960190</v>
       </c>
       <c r="E9" t="s">
@@ -2230,19 +2525,19 @@
         <f t="shared" si="0"/>
         <v>880.518401196019</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="Q9" s="14" t="s">
+      <c r="Q9" s="11" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
+      <c r="B10" s="11"/>
       <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>882168945719049</v>
       </c>
       <c r="E10" t="s">
@@ -2252,19 +2547,19 @@
         <f t="shared" si="0"/>
         <v>88.216894571904902</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="Q10" s="14" t="s">
+      <c r="Q10" s="11" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
+      <c r="B11" s="11"/>
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>8841131224288750</v>
       </c>
       <c r="E11" t="s">
@@ -2274,19 +2569,19 @@
         <f t="shared" si="0"/>
         <v>884.11312242887504</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="11" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
+      <c r="B12" s="11"/>
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>8863735604912900</v>
       </c>
       <c r="E12" t="s">
@@ -2296,19 +2591,19 @@
         <f t="shared" si="0"/>
         <v>886.37356049129005</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="Q12" s="11" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
+      <c r="B13" s="11"/>
       <c r="C13">
         <v>12</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>888972710906638</v>
       </c>
       <c r="E13" t="s">
@@ -2318,19 +2613,19 @@
         <f t="shared" si="0"/>
         <v>88.897271090663807</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="Q13" s="14" t="s">
+      <c r="Q13" s="11" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
+      <c r="B14" s="11"/>
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>8919328620696300</v>
       </c>
       <c r="E14" t="s">
@@ -2340,19 +2635,19 @@
         <f t="shared" si="0"/>
         <v>891.93286206963</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="Q14" s="14" t="s">
+      <c r="Q14" s="11" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B15" s="14"/>
+      <c r="B15" s="11"/>
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="12">
         <v>8952761531591410</v>
       </c>
       <c r="E15" t="s">
@@ -2362,19 +2657,19 @@
         <f t="shared" si="0"/>
         <v>895.27615315914102</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="Q15" s="14" t="s">
+      <c r="Q15" s="11" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B16" s="14"/>
+      <c r="B16" s="11"/>
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="12">
         <v>8990245858055180</v>
       </c>
       <c r="E16" t="s">
@@ -2384,19 +2679,19 @@
         <f t="shared" si="0"/>
         <v>899.02458580551797</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="Q16" s="11" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B17" s="14"/>
+      <c r="B17" s="11"/>
       <c r="C17">
         <v>16</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="12">
         <v>9032000343683710</v>
       </c>
       <c r="E17" t="s">
@@ -2406,19 +2701,19 @@
         <f t="shared" si="0"/>
         <v>903.20003436837101</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="14" t="s">
+      <c r="Q17" s="11" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B18" s="14"/>
+      <c r="B18" s="11"/>
       <c r="C18">
         <v>17</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="12">
         <v>9078242550774760</v>
       </c>
       <c r="E18" t="s">
@@ -2428,19 +2723,19 @@
         <f t="shared" si="0"/>
         <v>907.82425507747598</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="Q18" s="14" t="s">
+      <c r="Q18" s="11" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B19" s="14"/>
+      <c r="B19" s="11"/>
       <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="12">
         <v>9129188942317860</v>
       </c>
       <c r="E19" t="s">
@@ -2450,19 +2745,19 @@
         <f t="shared" si="0"/>
         <v>912.918894231786</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Q19" s="14" t="s">
+      <c r="Q19" s="11" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B20" s="14"/>
+      <c r="B20" s="11"/>
       <c r="C20">
         <v>19</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="12">
         <v>918505495609387</v>
       </c>
       <c r="E20" t="s">
@@ -2472,19 +2767,19 @@
         <f t="shared" si="0"/>
         <v>91.850549560938703</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="Q20" s="14" t="s">
+      <c r="Q20" s="11" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B21" s="14"/>
+      <c r="B21" s="11"/>
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>9246055072097910</v>
       </c>
       <c r="E21" t="s">
@@ -2494,19 +2789,19 @@
         <f t="shared" si="0"/>
         <v>924.60550720979097</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="Q21" s="14" t="s">
+      <c r="Q21" s="11" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B22" s="14"/>
+      <c r="B22" s="11"/>
       <c r="C22">
         <v>21</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="12">
         <v>9312402874261980</v>
       </c>
       <c r="E22" t="s">
@@ -2516,19 +2811,19 @@
         <f t="shared" si="0"/>
         <v>931.24028742619805</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="Q22" s="14" t="s">
+      <c r="Q22" s="11" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B23" s="14"/>
+      <c r="B23" s="11"/>
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="12">
         <v>938431110727126</v>
       </c>
       <c r="E23" t="s">
@@ -2544,56 +2839,56 @@
       <c r="H23" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Q23" s="14" t="s">
+      <c r="Q23" s="11" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B24" s="14"/>
+      <c r="B24" s="11"/>
       <c r="C24">
         <v>23</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="12">
         <v>9461991729127480</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="12">
         <v>1013065326633160</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="13">
         <f>D24/100000000000000</f>
         <v>94.619917291274803</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="13">
         <f>E24/1000000000000000</f>
         <v>1.01306532663316</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="13">
         <f>G24*3.6</f>
         <v>3.6470351758793758</v>
       </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="17" t="s">
+      <c r="I24" s="13"/>
+      <c r="J24" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="Q24" s="16" t="s">
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="Q24" s="13" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B25" s="14"/>
+      <c r="B25" s="11"/>
       <c r="C25">
         <v>24</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="12">
         <v>9545655960003930</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="12">
         <v>1.05276381909547E+16</v>
       </c>
       <c r="F25">
@@ -2608,22 +2903,22 @@
         <f t="shared" ref="H25:H88" si="1">G25*3.6</f>
         <v>3.7899497487436919</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="Q25" s="14" t="s">
+      <c r="Q25" s="11" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B26" s="14"/>
+      <c r="B26" s="11"/>
       <c r="C26">
         <v>25</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="12">
         <v>963551432785351</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="12">
         <v>1092462311557780</v>
       </c>
       <c r="F26">
@@ -2638,22 +2933,22 @@
         <f t="shared" si="1"/>
         <v>3.9328643216080081</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="Q26" s="14" t="s">
+      <c r="Q26" s="11" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B27" s="14"/>
+      <c r="B27" s="11"/>
       <c r="C27">
         <v>26</v>
       </c>
-      <c r="D27" s="15">
+      <c r="D27" s="12">
         <v>9731776711171170</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="12">
         <v>1.1321608040201E+16</v>
       </c>
       <c r="F27">
@@ -2668,22 +2963,22 @@
         <f t="shared" si="1"/>
         <v>40.7577889447236</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="Q27" s="14" t="s">
+      <c r="Q27" s="11" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B28" s="14"/>
+      <c r="B28" s="11"/>
       <c r="C28">
         <v>27</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="12">
         <v>98346523792724</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="12">
         <v>1.17185929648241E+16</v>
       </c>
       <c r="F28">
@@ -2698,22 +2993,22 @@
         <f t="shared" si="1"/>
         <v>42.186934673366764</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="J28" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="Q28" s="14" t="s">
+      <c r="Q28" s="11" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B29" s="14"/>
+      <c r="B29" s="11"/>
       <c r="C29">
         <v>28</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="12">
         <v>9944350030431820</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="12">
         <v>1.21155778894472E+16</v>
       </c>
       <c r="F29">
@@ -2728,22 +3023,22 @@
         <f t="shared" si="1"/>
         <v>43.616080402009921</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="Q29" s="14" t="s">
+      <c r="Q29" s="11" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B30" s="14"/>
+      <c r="B30" s="11"/>
       <c r="C30">
         <v>29</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="12">
         <v>1.00610778282316E+16</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="12">
         <v>1.25125628140703E+16</v>
       </c>
       <c r="F30">
@@ -2758,22 +3053,22 @@
         <f t="shared" si="1"/>
         <v>45.045226130653084</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="Q30" s="14" t="s">
+      <c r="Q30" s="11" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B31" s="14"/>
+      <c r="B31" s="11"/>
       <c r="C31">
         <v>30</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="12">
         <v>1.01850434365002E+16</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="12">
         <v>1.29095477386934E+16</v>
       </c>
       <c r="F31">
@@ -2788,22 +3083,22 @@
         <f t="shared" si="1"/>
         <v>46.474371859296241</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="Q31" s="14" t="s">
+      <c r="Q31" s="11" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B32" s="14"/>
+      <c r="B32" s="11"/>
       <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="12">
         <v>1031645405328100</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="12">
         <v>1.33065326633165E+16</v>
       </c>
       <c r="F32">
@@ -2818,22 +3113,22 @@
         <f t="shared" si="1"/>
         <v>47.903517587939398</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="Q32" s="14" t="s">
+      <c r="Q32" s="11" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B33" s="14"/>
+      <c r="B33" s="11"/>
       <c r="C33">
         <v>32</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="12">
         <v>1.04555164443609E+16</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="12">
         <v>137035175879397</v>
       </c>
       <c r="F33">
@@ -2848,22 +3143,22 @@
         <f t="shared" si="1"/>
         <v>0.49332663316582925</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="Q33" s="14" t="s">
+      <c r="Q33" s="11" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B34" s="14"/>
+      <c r="B34" s="11"/>
       <c r="C34">
         <v>33</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="12">
         <v>1.06024369770116E+16</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="12">
         <v>1.41005025125628E+16</v>
       </c>
       <c r="F34">
@@ -2878,22 +3173,22 @@
         <f t="shared" si="1"/>
         <v>50.76180904522608</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="Q34" s="14" t="s">
+      <c r="Q34" s="11" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B35" s="14"/>
+      <c r="B35" s="11"/>
       <c r="C35">
         <v>34</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="12">
         <v>1.0757421654749E+16</v>
       </c>
-      <c r="E35" s="15">
+      <c r="E35" s="12">
         <v>1.44974874371859E+16</v>
       </c>
       <c r="F35">
@@ -2908,53 +3203,53 @@
         <f t="shared" si="1"/>
         <v>52.190954773869237</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="Q35" s="14" t="s">
+      <c r="Q35" s="11" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B36" s="14"/>
+      <c r="B36" s="11"/>
       <c r="C36">
         <v>35</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="12">
         <v>1.09206761541059E+16</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="12">
         <v>1.4894472361809E+16</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="13">
         <f>D36/100000000000000</f>
         <v>109.206761541059</v>
       </c>
-      <c r="G36" s="16">
+      <c r="G36" s="13">
         <f>E36/10000000000000000</f>
         <v>1.4894472361808999</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36" s="13">
         <f t="shared" si="1"/>
         <v>5.3620100502512402</v>
       </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="17" t="s">
+      <c r="I36" s="13"/>
+      <c r="J36" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="Q36" s="16" t="s">
+      <c r="Q36" s="13" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B37" s="14"/>
+      <c r="B37" s="11"/>
       <c r="C37">
         <v>36</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="12">
         <v>1.10924058646258E+16</v>
       </c>
-      <c r="E37" s="15">
+      <c r="E37" s="12">
         <v>1.52914572864321E+16</v>
       </c>
       <c r="F37">
@@ -2969,22 +3264,22 @@
         <f t="shared" si="1"/>
         <v>55.049246231155564</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Q37" s="14" t="s">
+      <c r="Q37" s="11" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B38" s="14"/>
+      <c r="B38" s="11"/>
       <c r="C38">
         <v>37</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="12">
         <v>1.12728159335281E+16</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="12">
         <v>1.56884422110552E+16</v>
       </c>
       <c r="F38">
@@ -2999,22 +3294,22 @@
         <f t="shared" si="1"/>
         <v>56.478391959798721</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="Q38" s="14" t="s">
+      <c r="Q38" s="11" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B39" s="14"/>
+      <c r="B39" s="11"/>
       <c r="C39">
         <v>38</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="12">
         <v>1146211131674900</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="12">
         <v>1.60854271356783E+16</v>
       </c>
       <c r="F39">
@@ -3029,22 +3324,22 @@
         <f t="shared" si="1"/>
         <v>57.907537688441884</v>
       </c>
-      <c r="J39" s="14" t="s">
+      <c r="J39" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="Q39" s="14" t="s">
+      <c r="Q39" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B40" s="14"/>
+      <c r="B40" s="11"/>
       <c r="C40">
         <v>39</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="12">
         <v>1.16604968383355E+16</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="12">
         <v>1.64824120603015E+16</v>
       </c>
       <c r="F40">
@@ -3059,22 +3354,22 @@
         <f t="shared" si="1"/>
         <v>59.336683417085396</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="Q40" s="14" t="s">
+      <c r="Q40" s="11" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B41" s="14"/>
+      <c r="B41" s="11"/>
       <c r="C41">
         <v>40</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="12">
         <v>1.18681772604392E+16</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="12">
         <v>1.68793969849246E+16</v>
       </c>
       <c r="F41">
@@ -3089,22 +3384,22 @@
         <f t="shared" si="1"/>
         <v>60.76582914572856</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="J41" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="Q41" s="14" t="s">
+      <c r="Q41" s="11" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B42" s="14"/>
+      <c r="B42" s="11"/>
       <c r="C42">
         <v>41</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="12">
         <v>1208535736642010</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="12">
         <v>1727638190954770</v>
       </c>
       <c r="F42">
@@ -3119,22 +3414,22 @@
         <f t="shared" si="1"/>
         <v>6.219497487437172</v>
       </c>
-      <c r="J42" s="14" t="s">
+      <c r="J42" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="Q42" s="14" t="s">
+      <c r="Q42" s="11" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B43" s="14"/>
+      <c r="B43" s="11"/>
       <c r="C43">
         <v>42</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="12">
         <v>1.23122420598244E+16</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="12">
         <v>1.76733668341708E+16</v>
       </c>
       <c r="F43">
@@ -3149,22 +3444,22 @@
         <f t="shared" si="1"/>
         <v>63.62412060301488</v>
       </c>
-      <c r="J43" s="14" t="s">
+      <c r="J43" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="Q43" s="14" t="s">
+      <c r="Q43" s="11" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B44" s="14"/>
+      <c r="B44" s="11"/>
       <c r="C44">
         <v>43</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="12">
         <v>1.25490364822224E+16</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="12">
         <v>1.80703517587939E+16</v>
       </c>
       <c r="F44">
@@ -3179,22 +3474,22 @@
         <f t="shared" si="1"/>
         <v>65.053266331658051</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="Q44" s="14" t="s">
+      <c r="Q44" s="11" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B45" s="14"/>
+      <c r="B45" s="11"/>
       <c r="C45">
         <v>44</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="12">
         <v>1.27959461530896E+16</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="12">
         <v>1.8467336683417E+16</v>
       </c>
       <c r="F45">
@@ -3209,22 +3504,22 @@
         <f t="shared" si="1"/>
         <v>66.482412060301201</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="J45" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="Q45" s="14" t="s">
+      <c r="Q45" s="11" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B46" s="14"/>
+      <c r="B46" s="11"/>
       <c r="C46">
         <v>45</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="12">
         <v>1.30531771350677E+16</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="12">
         <v>1.88643216080402E+16</v>
       </c>
       <c r="F46">
@@ -3239,22 +3534,22 @@
         <f t="shared" si="1"/>
         <v>67.91155778894472</v>
       </c>
-      <c r="J46" s="14" t="s">
+      <c r="J46" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="Q46" s="14" t="s">
+      <c r="Q46" s="11" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B47" s="14"/>
+      <c r="B47" s="11"/>
       <c r="C47">
         <v>46</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D47" s="12">
         <v>1.33209362280579E+16</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="12">
         <v>1.92613065326633E+16</v>
       </c>
       <c r="F47">
@@ -3269,22 +3564,22 @@
         <f t="shared" si="1"/>
         <v>69.340703517587883</v>
       </c>
-      <c r="J47" s="14" t="s">
+      <c r="J47" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="Q47" s="14" t="s">
+      <c r="Q47" s="11" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B48" s="14"/>
+      <c r="B48" s="11"/>
       <c r="C48">
         <v>47</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="12">
         <v>1.35994311956576E+16</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="12">
         <v>1.96582914572864E+16</v>
       </c>
       <c r="F48">
@@ -3299,53 +3594,53 @@
         <f t="shared" si="1"/>
         <v>70.769849246231033</v>
       </c>
-      <c r="J48" s="14" t="s">
+      <c r="J48" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="Q48" s="14" t="s">
+      <c r="Q48" s="11" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B49" s="14"/>
+      <c r="B49" s="11"/>
       <c r="C49">
         <v>48</v>
       </c>
-      <c r="D49" s="15">
+      <c r="D49" s="12">
         <v>1.38888710274706E+16</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="12">
         <v>2005527638190950</v>
       </c>
-      <c r="F49" s="16">
+      <c r="F49" s="13">
         <f>D49/100000000000000</f>
         <v>138.888710274706</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="13">
         <f t="shared" si="2"/>
         <v>2.0055276381909501</v>
       </c>
-      <c r="H49" s="16">
+      <c r="H49" s="13">
         <f t="shared" si="1"/>
         <v>7.2198994974874209</v>
       </c>
-      <c r="I49" s="16"/>
-      <c r="J49" s="17" t="s">
+      <c r="I49" s="13"/>
+      <c r="J49" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="Q49" s="16" t="s">
+      <c r="Q49" s="13" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B50" s="14"/>
+      <c r="B50" s="11"/>
       <c r="C50">
         <v>49</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="12">
         <v>1418946624077840</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="12">
         <v>2.04522613065326E+16</v>
       </c>
       <c r="F50">
@@ -3360,22 +3655,22 @@
         <f t="shared" si="1"/>
         <v>73.62814070351736</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="J50" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="Q50" s="14" t="s">
+      <c r="Q50" s="11" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B51" s="14"/>
+      <c r="B51" s="11"/>
       <c r="C51">
         <v>50</v>
       </c>
-      <c r="D51" s="15">
+      <c r="D51" s="12">
         <v>1.45014292249736E+16</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="12">
         <v>2084924623115570</v>
       </c>
       <c r="F51">
@@ -3390,22 +3685,22 @@
         <f t="shared" si="1"/>
         <v>7.5057286432160515</v>
       </c>
-      <c r="J51" s="14" t="s">
+      <c r="J51" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="Q51" s="14" t="s">
+      <c r="Q51" s="11" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B52" s="14"/>
+      <c r="B52" s="11"/>
       <c r="C52">
         <v>51</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="12">
         <v>1482497463201660</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="12">
         <v>2.12462311557788E+16</v>
       </c>
       <c r="F52">
@@ -3420,22 +3715,22 @@
         <f t="shared" si="1"/>
         <v>76.486432160803687</v>
       </c>
-      <c r="J52" s="14" t="s">
+      <c r="J52" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="Q52" s="14" t="s">
+      <c r="Q52" s="11" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B53" s="14"/>
+      <c r="B53" s="11"/>
       <c r="C53">
         <v>52</v>
       </c>
-      <c r="D53" s="15">
+      <c r="D53" s="12">
         <v>1.51603198159934E+16</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="12">
         <v>2164321608040200</v>
       </c>
       <c r="F53">
@@ -3450,22 +3745,22 @@
         <f t="shared" si="1"/>
         <v>7.7915577889447203</v>
       </c>
-      <c r="J53" s="14" t="s">
+      <c r="J53" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Q53" s="14" t="s">
+      <c r="Q53" s="11" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B54" s="14"/>
+      <c r="B54" s="11"/>
       <c r="C54">
         <v>53</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D54" s="12">
         <v>1.55076853246232E+16</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="12">
         <v>2204020100502510</v>
       </c>
       <c r="F54">
@@ -3480,22 +3775,22 @@
         <f t="shared" si="1"/>
         <v>7.9344723618090365</v>
       </c>
-      <c r="J54" s="14" t="s">
+      <c r="J54" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="Q54" s="14" t="s">
+      <c r="Q54" s="11" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B55" s="14"/>
+      <c r="B55" s="11"/>
       <c r="C55">
         <v>54</v>
       </c>
-      <c r="D55" s="15">
+      <c r="D55" s="12">
         <v>1.58672954453016E+16</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="12">
         <v>2.24371859296482E+16</v>
       </c>
       <c r="F55">
@@ -3510,22 +3805,22 @@
         <f t="shared" si="1"/>
         <v>80.773869346733534</v>
       </c>
-      <c r="J55" s="14" t="s">
+      <c r="J55" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="Q55" s="14" t="s">
+      <c r="Q55" s="11" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B56" s="14"/>
+      <c r="B56" s="11"/>
       <c r="C56">
         <v>55</v>
       </c>
-      <c r="D56" s="15">
+      <c r="D56" s="12">
         <v>1.62393788079666E+16</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="12">
         <v>2.28341708542713E+16</v>
       </c>
       <c r="F56">
@@ -3540,22 +3835,22 @@
         <f t="shared" si="1"/>
         <v>82.203015075376683</v>
       </c>
-      <c r="J56" s="14" t="s">
+      <c r="J56" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="Q56" s="14" t="s">
+      <c r="Q56" s="11" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B57" s="14"/>
+      <c r="B57" s="11"/>
       <c r="C57">
         <v>56</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="12">
         <v>166241690467524</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="12">
         <v>2.32311557788944E+16</v>
       </c>
       <c r="F57">
@@ -3570,22 +3865,22 @@
         <f t="shared" si="1"/>
         <v>83.632160804019847</v>
       </c>
-      <c r="J57" s="14" t="s">
+      <c r="J57" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="Q57" s="14" t="s">
+      <c r="Q57" s="11" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B58" s="14"/>
+      <c r="B58" s="11"/>
       <c r="C58">
         <v>57</v>
       </c>
-      <c r="D58" s="15">
+      <c r="D58" s="12">
         <v>1.70219055220501E+16</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="12">
         <v>2362814070351750</v>
       </c>
       <c r="F58">
@@ -3600,22 +3895,22 @@
         <f t="shared" si="1"/>
         <v>8.5061306532663004</v>
       </c>
-      <c r="J58" s="14" t="s">
+      <c r="J58" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="Q58" s="14" t="s">
+      <c r="Q58" s="11" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B59" s="14"/>
+      <c r="B59" s="11"/>
       <c r="C59">
         <v>58</v>
       </c>
-      <c r="D59" s="15">
+      <c r="D59" s="12">
         <v>1.74328341042382E+16</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="12">
         <v>2.40251256281407E+16</v>
       </c>
       <c r="F59">
@@ -3630,22 +3925,22 @@
         <f t="shared" si="1"/>
         <v>86.490452261306515</v>
       </c>
-      <c r="J59" s="14" t="s">
+      <c r="J59" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="Q59" s="14" t="s">
+      <c r="Q59" s="11" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B60" s="14"/>
+      <c r="B60" s="11"/>
       <c r="C60">
         <v>59</v>
       </c>
-      <c r="D60" s="15">
+      <c r="D60" s="12">
         <v>1.78572080199738E+16</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="12">
         <v>2442211055276380</v>
       </c>
       <c r="F60">
@@ -3660,53 +3955,53 @@
         <f t="shared" si="1"/>
         <v>8.7919597989949683</v>
       </c>
-      <c r="J60" s="14" t="s">
+      <c r="J60" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="Q60" s="14" t="s">
+      <c r="Q60" s="11" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="61" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B61" s="14"/>
+      <c r="B61" s="11"/>
       <c r="C61">
         <v>60</v>
       </c>
-      <c r="D61" s="15">
+      <c r="D61" s="12">
         <v>1.82952887615695E+16</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E61" s="12">
         <v>2.48190954773869E+16</v>
       </c>
-      <c r="F61" s="16">
+      <c r="F61" s="13">
         <f>D61/100000000000000</f>
         <v>182.952887615695</v>
       </c>
-      <c r="G61" s="16">
+      <c r="G61" s="13">
         <f>E61/10000000000000000</f>
         <v>2.4819095477386899</v>
       </c>
-      <c r="H61" s="16">
+      <c r="H61" s="13">
         <f t="shared" si="1"/>
         <v>8.9348743718592836</v>
       </c>
-      <c r="I61" s="16"/>
-      <c r="J61" s="17" t="s">
+      <c r="I61" s="13"/>
+      <c r="J61" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="Q61" s="16" t="s">
+      <c r="Q61" s="13" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="62" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B62" s="14"/>
+      <c r="B62" s="11"/>
       <c r="C62">
         <v>61</v>
       </c>
-      <c r="D62" s="15">
+      <c r="D62" s="12">
         <v>1874734705960680</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="12">
         <v>2.521608040201E+16</v>
       </c>
       <c r="F62">
@@ -3721,22 +4016,22 @@
         <f t="shared" si="1"/>
         <v>90.777889447236007</v>
       </c>
-      <c r="J62" s="14" t="s">
+      <c r="J62" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q62" s="14" t="s">
+      <c r="Q62" s="11" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B63" s="14"/>
+      <c r="B63" s="11"/>
       <c r="C63">
         <v>62</v>
       </c>
-      <c r="D63" s="15">
+      <c r="D63" s="12">
         <v>1921366391857900</v>
       </c>
-      <c r="E63" s="15">
+      <c r="E63" s="12">
         <v>2.56130653266331E+16</v>
       </c>
       <c r="F63">
@@ -3751,22 +4046,22 @@
         <f t="shared" si="1"/>
         <v>92.20703517587917</v>
       </c>
-      <c r="J63" s="14" t="s">
+      <c r="J63" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="Q63" s="14" t="s">
+      <c r="Q63" s="11" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B64" s="14"/>
+      <c r="B64" s="11"/>
       <c r="C64">
         <v>63</v>
       </c>
-      <c r="D64" s="15">
+      <c r="D64" s="12">
         <v>1969453171500230</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="12">
         <v>2.60100502512562E+16</v>
       </c>
       <c r="F64">
@@ -3781,22 +4076,22 @@
         <f t="shared" si="1"/>
         <v>93.63618090452232</v>
       </c>
-      <c r="J64" s="14" t="s">
+      <c r="J64" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="Q64" s="14" t="s">
+      <c r="Q64" s="11" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="65" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B65" s="14"/>
+      <c r="B65" s="11"/>
       <c r="C65">
         <v>64</v>
       </c>
-      <c r="D65" s="15">
+      <c r="D65" s="12">
         <v>2.01902553570988E+16</v>
       </c>
-      <c r="E65" s="15">
+      <c r="E65" s="12">
         <v>264070351758794</v>
       </c>
       <c r="F65">
@@ -3811,22 +4106,22 @@
         <f t="shared" si="1"/>
         <v>0.95065326633165848</v>
       </c>
-      <c r="J65" s="14" t="s">
+      <c r="J65" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="Q65" s="14" t="s">
+      <c r="Q65" s="11" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="66" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B66" s="14"/>
+      <c r="B66" s="11"/>
       <c r="C66">
         <v>65</v>
       </c>
-      <c r="D66" s="15">
+      <c r="D66" s="12">
         <v>2070115350483560</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="12">
         <v>2.68040201005025E+16</v>
       </c>
       <c r="F66">
@@ -3841,22 +4136,22 @@
         <f t="shared" si="1"/>
         <v>96.494472361809002</v>
       </c>
-      <c r="J66" s="14" t="s">
+      <c r="J66" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="Q66" s="14" t="s">
+      <c r="Q66" s="11" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="67" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B67" s="14"/>
+      <c r="B67" s="11"/>
       <c r="C67">
         <v>66</v>
       </c>
-      <c r="D67" s="15">
+      <c r="D67" s="12">
         <v>2.12275598488093E+16</v>
       </c>
-      <c r="E67" s="15">
+      <c r="E67" s="12">
         <v>2720100502512560</v>
       </c>
       <c r="F67">
@@ -3871,22 +4166,22 @@
         <f t="shared" si="1"/>
         <v>9.7923618090452162</v>
       </c>
-      <c r="J67" s="14" t="s">
+      <c r="J67" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="Q67" s="14" t="s">
+      <c r="Q67" s="11" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="68" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B68" s="14"/>
+      <c r="B68" s="11"/>
       <c r="C68">
         <v>67</v>
       </c>
-      <c r="D68" s="15">
+      <c r="D68" s="12">
         <v>2.17698244461868E+16</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E68" s="12">
         <v>2.75979899497487E+16</v>
       </c>
       <c r="F68">
@@ -3901,22 +4196,22 @@
         <f t="shared" si="1"/>
         <v>99.35276381909533</v>
       </c>
-      <c r="J68" s="14" t="s">
+      <c r="J68" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q68" s="14" t="s">
+      <c r="Q68" s="11" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B69" s="14"/>
+      <c r="B69" s="11"/>
       <c r="C69">
         <v>68</v>
       </c>
-      <c r="D69" s="15">
+      <c r="D69" s="12">
         <v>2.23283151116675E+16</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="12">
         <v>2.79949748743718E+16</v>
       </c>
       <c r="F69">
@@ -3931,22 +4226,22 @@
         <f t="shared" si="1"/>
         <v>100.78190954773848</v>
       </c>
-      <c r="J69" s="14" t="s">
+      <c r="J69" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="Q69" s="14" t="s">
+      <c r="Q69" s="11" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B70" s="14"/>
+      <c r="B70" s="11"/>
       <c r="C70">
         <v>69</v>
       </c>
-      <c r="D70" s="15">
+      <c r="D70" s="12">
         <v>22903418861203</v>
       </c>
-      <c r="E70" s="15">
+      <c r="E70" s="12">
         <v>2.83919597989949E+16</v>
       </c>
       <c r="F70">
@@ -3961,22 +4256,22 @@
         <f t="shared" si="1"/>
         <v>102.21105527638164</v>
       </c>
-      <c r="J70" s="14" t="s">
+      <c r="J70" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="Q70" s="14" t="s">
+      <c r="Q70" s="11" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="71" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B71" s="14"/>
+      <c r="B71" s="11"/>
       <c r="C71">
         <v>70</v>
       </c>
-      <c r="D71" s="15">
+      <c r="D71" s="12">
         <v>2.34955434060181E+16</v>
       </c>
-      <c r="E71" s="15">
+      <c r="E71" s="12">
         <v>2878894472361800</v>
       </c>
       <c r="F71">
@@ -3991,22 +4286,22 @@
         <f t="shared" si="1"/>
         <v>10.364020100502481</v>
       </c>
-      <c r="J71" s="14" t="s">
+      <c r="J71" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="Q71" s="14" t="s">
+      <c r="Q71" s="11" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="72" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B72" s="14"/>
+      <c r="B72" s="11"/>
       <c r="C72">
         <v>71</v>
       </c>
-      <c r="D72" s="15">
+      <c r="D72" s="12">
         <v>2.41051186943009E+16</v>
       </c>
-      <c r="E72" s="15">
+      <c r="E72" s="12">
         <v>2918592964824120</v>
       </c>
       <c r="F72">
@@ -4021,22 +4316,22 @@
         <f t="shared" si="1"/>
         <v>10.506934673366832</v>
       </c>
-      <c r="J72" s="14" t="s">
+      <c r="J72" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="Q72" s="14" t="s">
+      <c r="Q72" s="11" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="73" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B73" s="14"/>
+      <c r="B73" s="11"/>
       <c r="C73">
         <v>72</v>
       </c>
-      <c r="D73" s="15">
+      <c r="D73" s="12">
         <v>2.47325984977867E+16</v>
       </c>
-      <c r="E73" s="15">
+      <c r="E73" s="12">
         <v>2.95829145728643E+16</v>
       </c>
       <c r="F73">
@@ -4051,53 +4346,53 @@
         <f t="shared" si="1"/>
         <v>106.49849246231149</v>
       </c>
-      <c r="J73" s="14" t="s">
+      <c r="J73" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="Q73" s="14" t="s">
+      <c r="Q73" s="11" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="74" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B74" s="14"/>
+      <c r="B74" s="11"/>
       <c r="C74">
         <v>73</v>
       </c>
-      <c r="D74" s="15">
+      <c r="D74" s="12">
         <v>2.53784620403452E+16</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="12">
         <v>2997989949748740</v>
       </c>
-      <c r="F74" s="16">
+      <c r="F74" s="13">
         <f>D74/100000000000000</f>
         <v>253.78462040345201</v>
       </c>
-      <c r="G74" s="16">
+      <c r="G74" s="13">
         <f t="shared" si="2"/>
         <v>2.9979899497487401</v>
       </c>
-      <c r="H74" s="16">
+      <c r="H74" s="13">
         <f t="shared" si="1"/>
         <v>10.792763819095464</v>
       </c>
-      <c r="I74" s="16"/>
-      <c r="J74" s="17" t="s">
+      <c r="I74" s="13"/>
+      <c r="J74" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="Q74" s="16" t="s">
+      <c r="Q74" s="13" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="75" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B75" s="14"/>
+      <c r="B75" s="11"/>
       <c r="C75">
         <v>74</v>
       </c>
-      <c r="D75" s="15">
+      <c r="D75" s="12">
         <v>2604321566558190</v>
       </c>
-      <c r="E75" s="15">
+      <c r="E75" s="12">
         <v>3.03768844221105E+16</v>
       </c>
       <c r="F75">
@@ -4112,22 +4407,22 @@
         <f t="shared" si="1"/>
         <v>109.3567839195978</v>
       </c>
-      <c r="J75" s="14" t="s">
+      <c r="J75" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="Q75" s="14" t="s">
+      <c r="Q75" s="11" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="76" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B76" s="14"/>
+      <c r="B76" s="11"/>
       <c r="C76">
         <v>75</v>
       </c>
-      <c r="D76" s="15">
+      <c r="D76" s="12">
         <v>2679285047448030</v>
       </c>
-      <c r="E76" s="15">
+      <c r="E76" s="12">
         <v>3077386934673360</v>
       </c>
       <c r="F76">
@@ -4142,22 +4437,22 @@
         <f t="shared" si="1"/>
         <v>11.078592964824097</v>
       </c>
-      <c r="J76" s="14" t="s">
+      <c r="J76" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="Q76" s="14" t="s">
+      <c r="Q76" s="11" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="77" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B77" s="14"/>
+      <c r="B77" s="11"/>
       <c r="C77">
         <v>76</v>
       </c>
-      <c r="D77" s="15">
+      <c r="D77" s="12">
         <v>2.74262153123724E+16</v>
       </c>
-      <c r="E77" s="15">
+      <c r="E77" s="12">
         <v>3.11708542713567E+16</v>
       </c>
       <c r="F77">
@@ -4172,22 +4467,22 @@
         <f t="shared" si="1"/>
         <v>112.21507537688412</v>
       </c>
-      <c r="J77" s="14" t="s">
+      <c r="J77" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="Q77" s="14" t="s">
+      <c r="Q77" s="11" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="78" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B78" s="14"/>
+      <c r="B78" s="11"/>
       <c r="C78">
         <v>77</v>
       </c>
-      <c r="D78" s="15">
+      <c r="D78" s="12">
         <v>2808308182841740</v>
       </c>
-      <c r="E78" s="15">
+      <c r="E78" s="12">
         <v>315678391959799</v>
       </c>
       <c r="F78">
@@ -4202,22 +4497,22 @@
         <f t="shared" si="1"/>
         <v>1.1364422110552765</v>
       </c>
-      <c r="J78" s="14" t="s">
+      <c r="J78" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="Q78" s="14" t="s">
+      <c r="Q78" s="11" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="79" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B79" s="14"/>
+      <c r="B79" s="11"/>
       <c r="C79">
         <v>78</v>
       </c>
-      <c r="D79" s="15">
+      <c r="D79" s="12">
         <v>2876429210196110</v>
       </c>
-      <c r="E79" s="15">
+      <c r="E79" s="12">
         <v>3.1964824120603E+16</v>
       </c>
       <c r="F79">
@@ -4232,22 +4527,22 @@
         <f t="shared" si="1"/>
         <v>115.07336683417081</v>
       </c>
-      <c r="J79" s="14" t="s">
+      <c r="J79" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="Q79" s="14" t="s">
+      <c r="Q79" s="11" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="80" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B80" s="14"/>
+      <c r="B80" s="11"/>
       <c r="C80">
         <v>79</v>
       </c>
-      <c r="D80" s="15">
+      <c r="D80" s="12">
         <v>2.94707807679066E+16</v>
       </c>
-      <c r="E80" s="15">
+      <c r="E80" s="12">
         <v>3.23618090452261E+16</v>
       </c>
       <c r="F80">
@@ -4262,22 +4557,22 @@
         <f t="shared" si="1"/>
         <v>116.50251256281398</v>
       </c>
-      <c r="J80" s="14" t="s">
+      <c r="J80" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="Q80" s="14" t="s">
+      <c r="Q80" s="11" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="81" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B81" s="14"/>
+      <c r="B81" s="11"/>
       <c r="C81">
         <v>80</v>
       </c>
-      <c r="D81" s="15">
+      <c r="D81" s="12">
         <v>3.0203584074669E+16</v>
       </c>
-      <c r="E81" s="15">
+      <c r="E81" s="12">
         <v>3.27587939698492E+16</v>
       </c>
       <c r="F81">
@@ -4292,22 +4587,22 @@
         <f t="shared" si="1"/>
         <v>117.93165829145713</v>
       </c>
-      <c r="J81" s="14" t="s">
+      <c r="J81" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="Q81" s="14" t="s">
+      <c r="Q81" s="11" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="82" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B82" s="14"/>
+      <c r="B82" s="11"/>
       <c r="C82">
         <v>81</v>
       </c>
-      <c r="D82" s="15">
+      <c r="D82" s="12">
         <v>309638504650558</v>
       </c>
-      <c r="E82" s="15">
+      <c r="E82" s="12">
         <v>3.31557788944723E+16</v>
       </c>
       <c r="F82">
@@ -4322,22 +4617,22 @@
         <f t="shared" si="1"/>
         <v>119.36080402010028</v>
       </c>
-      <c r="J82" s="14" t="s">
+      <c r="J82" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="Q82" s="14" t="s">
+      <c r="Q82" s="11" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="83" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B83" s="14"/>
+      <c r="B83" s="11"/>
       <c r="C83">
         <v>82</v>
       </c>
-      <c r="D83" s="15">
+      <c r="D83" s="12">
         <v>3175285280780760</v>
       </c>
-      <c r="E83" s="15">
+      <c r="E83" s="12">
         <v>3355276381909540</v>
       </c>
       <c r="F83">
@@ -4352,22 +4647,22 @@
         <f t="shared" si="1"/>
         <v>12.078994974874345</v>
       </c>
-      <c r="J83" s="14" t="s">
+      <c r="J83" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="Q83" s="14" t="s">
+      <c r="Q83" s="11" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="84" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B84" s="14"/>
+      <c r="B84" s="11"/>
       <c r="C84">
         <v>83</v>
       </c>
-      <c r="D84" s="15">
+      <c r="D84" s="12">
         <v>3.25720024263476E+16</v>
       </c>
-      <c r="E84" s="15">
+      <c r="E84" s="12">
         <v>3.39497487437185E+16</v>
       </c>
       <c r="F84">
@@ -4382,22 +4677,22 @@
         <f t="shared" si="1"/>
         <v>122.2190954773866</v>
       </c>
-      <c r="J84" s="14" t="s">
+      <c r="J84" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="Q84" s="14" t="s">
+      <c r="Q84" s="11" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="85" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B85" s="14"/>
+      <c r="B85" s="11"/>
       <c r="C85">
         <v>84</v>
       </c>
-      <c r="D85" s="15">
+      <c r="D85" s="12">
         <v>3.34228650891382E+16</v>
       </c>
-      <c r="E85" s="15">
+      <c r="E85" s="12">
         <v>3434673366834170</v>
       </c>
       <c r="F85">
@@ -4412,22 +4707,22 @@
         <f t="shared" si="1"/>
         <v>12.364824120603011</v>
       </c>
-      <c r="J85" s="14" t="s">
+      <c r="J85" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="Q85" s="14" t="s">
+      <c r="Q85" s="11" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="86" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B86" s="14"/>
+      <c r="B86" s="11"/>
       <c r="C86">
         <v>85</v>
       </c>
-      <c r="D86" s="15">
+      <c r="D86" s="12">
         <v>3.4307179142964E+16</v>
       </c>
-      <c r="E86" s="15">
+      <c r="E86" s="12">
         <v>3.47437185929648E+16</v>
       </c>
       <c r="F86">
@@ -4442,53 +4737,53 @@
         <f t="shared" si="1"/>
         <v>125.07738693467327</v>
       </c>
-      <c r="J86" s="14" t="s">
+      <c r="J86" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="Q86" s="14" t="s">
+      <c r="Q86" s="11" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="87" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B87" s="14"/>
+      <c r="B87" s="11"/>
       <c r="C87">
         <v>86</v>
       </c>
-      <c r="D87" s="15">
+      <c r="D87" s="12">
         <v>3.52268759863408E+16</v>
       </c>
-      <c r="E87" s="15">
+      <c r="E87" s="12">
         <v>3.51407035175879E+16</v>
       </c>
-      <c r="F87" s="16">
+      <c r="F87" s="13">
         <f>D87/100000000000000</f>
         <v>352.26875986340798</v>
       </c>
-      <c r="G87" s="16">
+      <c r="G87" s="13">
         <f>E87/10000000000000000</f>
         <v>3.5140703517587899</v>
       </c>
-      <c r="H87" s="16">
+      <c r="H87" s="13">
         <f t="shared" si="1"/>
         <v>12.650653266331643</v>
       </c>
-      <c r="I87" s="16"/>
-      <c r="J87" s="17" t="s">
+      <c r="I87" s="13"/>
+      <c r="J87" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="Q87" s="16" t="s">
+      <c r="Q87" s="13" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="88" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B88" s="14"/>
+      <c r="B88" s="11"/>
       <c r="C88">
         <v>87</v>
       </c>
-      <c r="D88" s="15">
+      <c r="D88" s="12">
         <v>3.61841030949232E+16</v>
       </c>
-      <c r="E88" s="15">
+      <c r="E88" s="12">
         <v>3.5537688442211E+16</v>
       </c>
       <c r="F88">
@@ -4503,22 +4798,22 @@
         <f t="shared" si="1"/>
         <v>127.9356783919596</v>
       </c>
-      <c r="J88" s="14" t="s">
+      <c r="J88" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="Q88" s="14" t="s">
+      <c r="Q88" s="11" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="89" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B89" s="14"/>
+      <c r="B89" s="11"/>
       <c r="C89">
         <v>88</v>
       </c>
-      <c r="D89" s="15">
+      <c r="D89" s="12">
         <v>371812498239675</v>
       </c>
-      <c r="E89" s="15">
+      <c r="E89" s="12">
         <v>3593467336683410</v>
       </c>
       <c r="F89">
@@ -4533,22 +4828,22 @@
         <f t="shared" ref="H89:H125" si="5">G89*3.6</f>
         <v>12.936482412060275</v>
       </c>
-      <c r="J89" s="14" t="s">
+      <c r="J89" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="Q89" s="14" t="s">
+      <c r="Q89" s="11" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="90" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B90" s="14"/>
+      <c r="B90" s="11"/>
       <c r="C90">
         <v>89</v>
       </c>
-      <c r="D90" s="15">
+      <c r="D90" s="12">
         <v>3822097622425910</v>
       </c>
-      <c r="E90" s="15">
+      <c r="E90" s="12">
         <v>3633165829145720</v>
       </c>
       <c r="F90">
@@ -4563,22 +4858,22 @@
         <f t="shared" si="5"/>
         <v>13.079396984924593</v>
       </c>
-      <c r="J90" s="14" t="s">
+      <c r="J90" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="Q90" s="14" t="s">
+      <c r="Q90" s="11" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B91" s="14"/>
+      <c r="B91" s="11"/>
       <c r="C91">
         <v>90</v>
       </c>
-      <c r="D91" s="15">
+      <c r="D91" s="12">
         <v>3930624511700120</v>
       </c>
-      <c r="E91" s="15">
+      <c r="E91" s="12">
         <v>3.67286432160804E+16</v>
       </c>
       <c r="F91">
@@ -4593,22 +4888,22 @@
         <f t="shared" si="5"/>
         <v>132.22311557788944</v>
       </c>
-      <c r="J91" s="14" t="s">
+      <c r="J91" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="Q91" s="14" t="s">
+      <c r="Q91" s="11" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B92" s="14"/>
+      <c r="B92" s="11"/>
       <c r="C92">
         <v>91</v>
       </c>
-      <c r="D92" s="15">
+      <c r="D92" s="12">
         <v>4.0440357679498304E+16</v>
       </c>
-      <c r="E92" s="15">
+      <c r="E92" s="12">
         <v>3712562814070350</v>
       </c>
       <c r="F92">
@@ -4623,22 +4918,22 @@
         <f t="shared" si="5"/>
         <v>13.36522613065326</v>
       </c>
-      <c r="J92" s="14" t="s">
+      <c r="J92" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="Q92" s="14" t="s">
+      <c r="Q92" s="11" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="93" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B93" s="14"/>
+      <c r="B93" s="11"/>
       <c r="C93">
         <v>92</v>
       </c>
-      <c r="D93" s="15">
+      <c r="D93" s="12">
         <v>416269927964812</v>
       </c>
-      <c r="E93" s="15">
+      <c r="E93" s="12">
         <v>3.75226130653266E+16</v>
       </c>
       <c r="F93">
@@ -4653,22 +4948,22 @@
         <f t="shared" si="5"/>
         <v>135.08140703517577</v>
       </c>
-      <c r="J93" s="14" t="s">
+      <c r="J93" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="Q93" s="14" t="s">
+      <c r="Q93" s="11" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="94" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B94" s="14"/>
+      <c r="B94" s="11"/>
       <c r="C94">
         <v>93</v>
       </c>
-      <c r="D94" s="15">
+      <c r="D94" s="12">
         <v>4287025043101230</v>
       </c>
-      <c r="E94" s="15">
+      <c r="E94" s="12">
         <v>3791959798994970</v>
       </c>
       <c r="F94">
@@ -4683,22 +4978,22 @@
         <f t="shared" si="5"/>
         <v>13.651055276381893</v>
       </c>
-      <c r="J94" s="14" t="s">
+      <c r="J94" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="Q94" s="14" t="s">
+      <c r="Q94" s="11" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="95" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B95" s="14"/>
+      <c r="B95" s="11"/>
       <c r="C95">
         <v>94</v>
       </c>
-      <c r="D95" s="15">
+      <c r="D95" s="12">
         <v>4417469926338350</v>
       </c>
-      <c r="E95" s="15">
+      <c r="E95" s="12">
         <v>3.83165829145728E+16</v>
       </c>
       <c r="F95">
@@ -4713,22 +5008,22 @@
         <f t="shared" si="5"/>
         <v>137.93969849246207</v>
       </c>
-      <c r="J95" s="14" t="s">
+      <c r="J95" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="Q95" s="14" t="s">
+      <c r="Q95" s="11" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="96" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B96" s="14"/>
+      <c r="B96" s="11"/>
       <c r="C96">
         <v>95</v>
       </c>
-      <c r="D96" s="15">
+      <c r="D96" s="12">
         <v>455454288355972</v>
       </c>
-      <c r="E96" s="15">
+      <c r="E96" s="12">
         <v>3871356783919590</v>
       </c>
       <c r="F96">
@@ -4743,22 +5038,22 @@
         <f t="shared" si="5"/>
         <v>13.936884422110525</v>
       </c>
-      <c r="J96" s="14" t="s">
+      <c r="J96" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="Q96" s="16" t="s">
+      <c r="Q96" s="13" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B97" s="14"/>
+      <c r="B97" s="11"/>
       <c r="C97">
         <v>96</v>
       </c>
-      <c r="D97" s="15">
+      <c r="D97" s="12">
         <v>4.6988106422155296E+16</v>
       </c>
-      <c r="E97" s="15">
+      <c r="E97" s="12">
         <v>391105527638191</v>
       </c>
       <c r="F97">
@@ -4773,19 +5068,19 @@
         <f t="shared" si="5"/>
         <v>1.4079798994974877</v>
       </c>
-      <c r="J97" s="14" t="s">
+      <c r="J97" s="11" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B98" s="14"/>
+      <c r="B98" s="11"/>
       <c r="C98">
         <v>97</v>
       </c>
-      <c r="D98" s="15">
+      <c r="D98" s="12">
         <v>4.8509038824222496E+16</v>
       </c>
-      <c r="E98" s="15">
+      <c r="E98" s="12">
         <v>3.95075376884422E+16</v>
       </c>
       <c r="F98">
@@ -4800,19 +5095,19 @@
         <f t="shared" si="5"/>
         <v>142.22713567839193</v>
       </c>
-      <c r="J98" s="14" t="s">
+      <c r="J98" s="11" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B99" s="14"/>
+      <c r="B99" s="11"/>
       <c r="C99">
         <v>98</v>
       </c>
-      <c r="D99" s="15">
+      <c r="D99" s="12">
         <v>5.0115239252969696E+16</v>
       </c>
-      <c r="E99" s="15">
+      <c r="E99" s="12">
         <v>3.9904522613065296E+16</v>
       </c>
       <c r="F99">
@@ -4827,47 +5122,47 @@
         <f t="shared" si="5"/>
         <v>143.65628140703507</v>
       </c>
-      <c r="J99" s="14" t="s">
+      <c r="J99" s="11" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B100" s="14"/>
+      <c r="B100" s="11"/>
       <c r="C100">
         <v>99</v>
       </c>
-      <c r="D100" s="15">
+      <c r="D100" s="12">
         <v>5181449942859220</v>
       </c>
-      <c r="E100" s="15">
+      <c r="E100" s="12">
         <v>4030150753768840</v>
       </c>
-      <c r="F100" s="16">
+      <c r="F100" s="13">
         <f t="shared" si="3"/>
         <v>518.14499428592205</v>
       </c>
-      <c r="G100" s="16">
+      <c r="G100" s="13">
         <f t="shared" si="4"/>
         <v>4.0301507537688401</v>
       </c>
-      <c r="H100" s="16">
+      <c r="H100" s="13">
         <f t="shared" si="5"/>
         <v>14.508542713567826</v>
       </c>
-      <c r="I100" s="16"/>
-      <c r="J100" s="17" t="s">
+      <c r="I100" s="13"/>
+      <c r="J100" s="14" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B101" s="14"/>
+      <c r="B101" s="11"/>
       <c r="C101">
         <v>100</v>
       </c>
-      <c r="D101" s="15">
+      <c r="D101" s="12">
         <v>5361546697403200</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E101" s="12">
         <v>4069849246231150</v>
       </c>
       <c r="F101">
@@ -4882,19 +5177,19 @@
         <f t="shared" si="5"/>
         <v>14.651457286432139</v>
       </c>
-      <c r="J101" s="14" t="s">
+      <c r="J101" s="11" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B102" s="14"/>
+      <c r="B102" s="11"/>
       <c r="C102">
         <v>101</v>
       </c>
-      <c r="D102" s="15">
+      <c r="D102" s="12">
         <v>5552772812187270</v>
       </c>
-      <c r="E102" s="15">
+      <c r="E102" s="12">
         <v>4109547738693460</v>
       </c>
       <c r="F102">
@@ -4909,19 +5204,19 @@
         <f t="shared" si="5"/>
         <v>14.794371859296458</v>
       </c>
-      <c r="J102" s="14" t="s">
+      <c r="J102" s="11" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B103" s="14"/>
+      <c r="B103" s="11"/>
       <c r="C103">
         <v>102</v>
       </c>
-      <c r="D103" s="15">
+      <c r="D103" s="12">
         <v>5756189567615800</v>
       </c>
-      <c r="E103" s="15">
+      <c r="E103" s="12">
         <v>4149246231155770</v>
       </c>
       <c r="F103">
@@ -4936,19 +5231,19 @@
         <f t="shared" si="5"/>
         <v>14.937286432160771</v>
       </c>
-      <c r="J103" s="14" t="s">
+      <c r="J103" s="11" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B104" s="14"/>
+      <c r="B104" s="11"/>
       <c r="C104">
         <v>103</v>
       </c>
-      <c r="D104" s="15">
+      <c r="D104" s="12">
         <v>5972970212959560</v>
       </c>
-      <c r="E104" s="15">
+      <c r="E104" s="12">
         <v>418894472361809</v>
       </c>
       <c r="F104">
@@ -4963,19 +5258,19 @@
         <f t="shared" si="5"/>
         <v>1.5080201005025125</v>
       </c>
-      <c r="J104" s="14" t="s">
+      <c r="J104" s="11" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B105" s="14"/>
+      <c r="B105" s="11"/>
       <c r="C105">
         <v>104</v>
       </c>
-      <c r="D105" s="15">
+      <c r="D105" s="12">
         <v>6204409782030830</v>
       </c>
-      <c r="E105" s="15">
+      <c r="E105" s="12">
         <v>4.2286432160804E+16</v>
       </c>
       <c r="F105">
@@ -4990,19 +5285,19 @@
         <f t="shared" si="5"/>
         <v>152.23115577889439</v>
       </c>
-      <c r="J105" s="14" t="s">
+      <c r="J105" s="11" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B106" s="14"/>
+      <c r="B106" s="11"/>
       <c r="C106">
         <v>105</v>
       </c>
-      <c r="D106" s="15">
+      <c r="D106" s="12">
         <v>6451935355767830</v>
       </c>
-      <c r="E106" s="15">
+      <c r="E106" s="12">
         <v>4268341708542710</v>
       </c>
       <c r="F106">
@@ -5017,19 +5312,19 @@
         <f t="shared" si="5"/>
         <v>15.366030150753756</v>
       </c>
-      <c r="J106" s="14" t="s">
+      <c r="J106" s="11" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B107" s="14"/>
+      <c r="B107" s="11"/>
       <c r="C107">
         <v>106</v>
       </c>
-      <c r="D107" s="15">
+      <c r="D107" s="12">
         <v>6717116647610960</v>
       </c>
-      <c r="E107" s="15">
+      <c r="E107" s="12">
         <v>4308040201005020</v>
       </c>
       <c r="F107">
@@ -5044,19 +5339,19 @@
         <f t="shared" si="5"/>
         <v>15.508944723618072</v>
       </c>
-      <c r="J107" s="14" t="s">
+      <c r="J107" s="11" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B108" s="14"/>
+      <c r="B108" s="11"/>
       <c r="C108">
         <v>107</v>
       </c>
-      <c r="D108" s="15">
+      <c r="D108" s="12">
         <v>7001677030195470</v>
       </c>
-      <c r="E108" s="15">
+      <c r="E108" s="12">
         <v>4.3477386934673296E+16</v>
       </c>
       <c r="F108">
@@ -5071,19 +5366,19 @@
         <f t="shared" si="5"/>
         <v>156.51859296482388</v>
       </c>
-      <c r="J108" s="14" t="s">
+      <c r="J108" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B109" s="14"/>
+      <c r="B109" s="11"/>
       <c r="C109">
         <v>108</v>
       </c>
-      <c r="D109" s="15">
+      <c r="D109" s="12">
         <v>7307505539104790</v>
       </c>
-      <c r="E109" s="15">
+      <c r="E109" s="12">
         <v>4387437185929640</v>
       </c>
       <c r="F109">
@@ -5098,19 +5393,19 @@
         <f t="shared" si="5"/>
         <v>15.794773869346704</v>
       </c>
-      <c r="J109" s="14" t="s">
+      <c r="J109" s="11" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B110" s="14"/>
+      <c r="B110" s="11"/>
       <c r="C110">
         <v>109</v>
       </c>
-      <c r="D110" s="15">
+      <c r="D110" s="12">
         <v>7636669031327530</v>
       </c>
-      <c r="E110" s="15">
+      <c r="E110" s="12">
         <v>4427135678391950</v>
       </c>
       <c r="F110">
@@ -5125,19 +5420,19 @@
         <f t="shared" si="5"/>
         <v>15.937688442211021</v>
       </c>
-      <c r="J110" s="14" t="s">
+      <c r="J110" s="11" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B111" s="14"/>
+      <c r="B111" s="11"/>
       <c r="C111">
         <v>110</v>
       </c>
-      <c r="D111" s="15">
+      <c r="D111" s="12">
         <v>7991420677821220</v>
       </c>
-      <c r="E111" s="15">
+      <c r="E111" s="12">
         <v>4466834170854270</v>
       </c>
       <c r="F111">
@@ -5152,44 +5447,44 @@
         <f t="shared" si="5"/>
         <v>16.080603015075372</v>
       </c>
-      <c r="J111" s="17" t="s">
+      <c r="J111" s="14" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B112" s="14"/>
+      <c r="B112" s="11"/>
       <c r="C112">
         <v>111</v>
       </c>
-      <c r="D112" s="15">
+      <c r="D112" s="12">
         <v>8374205619801580</v>
       </c>
-      <c r="E112" s="15">
+      <c r="E112" s="12">
         <v>4506532663316580</v>
       </c>
-      <c r="F112" s="16">
+      <c r="F112" s="13">
         <f t="shared" si="3"/>
         <v>837.42056198015803</v>
       </c>
-      <c r="G112" s="16">
+      <c r="G112" s="13">
         <f t="shared" si="4"/>
         <v>4.5065326633165803</v>
       </c>
-      <c r="H112" s="16">
+      <c r="H112" s="13">
         <f t="shared" si="5"/>
         <v>16.223517587939689</v>
       </c>
-      <c r="I112" s="16"/>
+      <c r="I112" s="13"/>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B113" s="14"/>
+      <c r="B113" s="11"/>
       <c r="C113">
         <v>112</v>
       </c>
-      <c r="D113" s="15">
+      <c r="D113" s="12">
         <v>8787681112441620</v>
       </c>
-      <c r="E113" s="15">
+      <c r="E113" s="12">
         <v>4546231155778890</v>
       </c>
       <c r="F113">
@@ -5206,14 +5501,14 @@
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B114" s="14"/>
+      <c r="B114" s="11"/>
       <c r="C114">
         <v>113</v>
       </c>
-      <c r="D114" s="15">
+      <c r="D114" s="12">
         <v>9234763213742290</v>
       </c>
-      <c r="E114" s="15">
+      <c r="E114" s="12">
         <v>4585929648241200</v>
       </c>
       <c r="F114">
@@ -5230,14 +5525,14 @@
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B115" s="14"/>
+      <c r="B115" s="11"/>
       <c r="C115">
         <v>114</v>
       </c>
-      <c r="D115" s="15">
+      <c r="D115" s="12">
         <v>9718646933033380</v>
       </c>
-      <c r="E115" s="15">
+      <c r="E115" s="12">
         <v>4625628140703510</v>
       </c>
       <c r="F115">
@@ -5254,14 +5549,14 @@
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B116" s="14"/>
+      <c r="B116" s="11"/>
       <c r="C116">
         <v>115</v>
       </c>
-      <c r="D116" s="15">
+      <c r="D116" s="12">
         <v>1.02427011220768E+16</v>
       </c>
-      <c r="E116" s="15">
+      <c r="E116" s="12">
         <v>4.66532663316582E+16</v>
       </c>
       <c r="F116">
@@ -5278,14 +5573,14 @@
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B117" s="14"/>
+      <c r="B117" s="11"/>
       <c r="C117">
         <v>116</v>
       </c>
-      <c r="D117" s="15">
+      <c r="D117" s="12">
         <v>1.08102924404888E+16</v>
       </c>
-      <c r="E117" s="15">
+      <c r="E117" s="12">
         <v>4705025125628140</v>
       </c>
       <c r="F117">
@@ -5302,14 +5597,14 @@
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B118" s="14"/>
+      <c r="B118" s="11"/>
       <c r="C118">
         <v>117</v>
       </c>
-      <c r="D118" s="15">
+      <c r="D118" s="12">
         <v>1.14248897065431E+16</v>
       </c>
-      <c r="E118" s="15">
+      <c r="E118" s="12">
         <v>4744723618090450</v>
       </c>
       <c r="F118">
@@ -5326,14 +5621,14 @@
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B119" s="14"/>
+      <c r="B119" s="11"/>
       <c r="C119">
         <v>118</v>
       </c>
-      <c r="D119" s="15">
+      <c r="D119" s="12">
         <v>1.20907396508144E+16</v>
       </c>
-      <c r="E119" s="15">
+      <c r="E119" s="12">
         <v>4784422110552760</v>
       </c>
       <c r="F119">
@@ -5350,14 +5645,14 @@
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B120" s="14"/>
+      <c r="B120" s="11"/>
       <c r="C120">
         <v>119</v>
       </c>
-      <c r="D120" s="15">
+      <c r="D120" s="12">
         <v>1.28136132776176E+16</v>
       </c>
-      <c r="E120" s="15">
+      <c r="E120" s="12">
         <v>4824120603015070</v>
       </c>
       <c r="F120">
@@ -5374,14 +5669,14 @@
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B121" s="14"/>
+      <c r="B121" s="11"/>
       <c r="C121">
         <v>120</v>
       </c>
-      <c r="D121" s="15">
+      <c r="D121" s="12">
         <v>1.36002857622891E+16</v>
       </c>
-      <c r="E121" s="15">
+      <c r="E121" s="12">
         <v>4863819095477380</v>
       </c>
       <c r="F121">
@@ -5398,14 +5693,14 @@
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B122" s="14"/>
+      <c r="B122" s="11"/>
       <c r="C122">
         <v>121</v>
       </c>
-      <c r="D122" s="15">
+      <c r="D122" s="12">
         <v>1445600133584770</v>
       </c>
-      <c r="E122" s="15">
+      <c r="E122" s="12">
         <v>4903517587939690</v>
       </c>
       <c r="F122">
@@ -5422,14 +5717,14 @@
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B123" s="14"/>
+      <c r="B123" s="11"/>
       <c r="C123">
         <v>122</v>
       </c>
-      <c r="D123" s="15">
+      <c r="D123" s="12">
         <v>1538156634613940</v>
       </c>
-      <c r="E123" s="15">
+      <c r="E123" s="12">
         <v>494321608040201</v>
       </c>
       <c r="F123">
@@ -5446,14 +5741,14 @@
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B124" s="14"/>
+      <c r="B124" s="11"/>
       <c r="C124">
         <v>123</v>
       </c>
-      <c r="D124" s="15">
+      <c r="D124" s="12">
         <v>1.63738775623294E+16</v>
       </c>
-      <c r="E124" s="15">
+      <c r="E124" s="12">
         <v>4982914572864320</v>
       </c>
       <c r="F124">
@@ -5470,35 +5765,35 @@
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B125" s="14"/>
+      <c r="B125" s="11"/>
       <c r="C125">
         <v>124</v>
       </c>
-      <c r="D125" s="15">
+      <c r="D125" s="12">
         <v>1.74324665596751E+16</v>
       </c>
-      <c r="E125" s="15">
+      <c r="E125" s="12">
         <v>5022613065326630</v>
       </c>
-      <c r="F125" s="16">
+      <c r="F125" s="13">
         <f t="shared" si="3"/>
         <v>1743.2466559675099</v>
       </c>
-      <c r="G125" s="16">
+      <c r="G125" s="13">
         <f t="shared" si="4"/>
         <v>5.0226130653266301</v>
       </c>
-      <c r="H125" s="16">
+      <c r="H125" s="13">
         <f t="shared" si="5"/>
         <v>18.081407035175868</v>
       </c>
-      <c r="I125" s="16"/>
+      <c r="I125" s="13"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B126" s="14"/>
+      <c r="B126" s="11"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B127" s="14"/>
+      <c r="B127" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>